<commit_message>
se actualizo diccionario de datos
</commit_message>
<xml_diff>
--- a/Diccionario de Datos/SexShop.xlsx
+++ b/Diccionario de Datos/SexShop.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sex shop\Diccionario de Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sex shop\Diccionario de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F30FBFA9-B592-4783-B35F-B4FFBCF54ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA2564B-121B-437E-813C-B93EED385125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="751" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2760,12 +2760,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>